<commit_message>
Updating hyperparameters and Readme.md
</commit_message>
<xml_diff>
--- a/hyper parameters.xlsx
+++ b/hyper parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I318768\Documents\Udacity\DL\Projects\Project 1\deep-learning-master_1\deep-learning-master\first-neural-network\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I318768\git\First-Neural-Network\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,10 +443,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>10000</v>
+        <v>11000</v>
       </c>
       <c r="B2">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="C2">
         <v>8</v>
@@ -455,115 +455,115 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>7.5999999999999998E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="F2">
-        <v>0.16300000000000001</v>
+        <v>0.13400000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>6000</v>
+        <v>11000</v>
       </c>
       <c r="B3">
         <v>0.3</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>0.10100000000000001</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="F3">
-        <v>0.20499999999999999</v>
+        <v>0.14099999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>6000</v>
+        <v>11000</v>
       </c>
       <c r="B4">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="C4">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>9.6000000000000002E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="F4">
-        <v>0.20699999999999999</v>
+        <v>0.14399999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="B5">
         <v>0.3</v>
       </c>
       <c r="C5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5">
-        <v>0.10199999999999999</v>
+        <v>6.2E-2</v>
       </c>
       <c r="F5">
-        <v>0.22700000000000001</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>6000</v>
+        <v>10000</v>
       </c>
       <c r="B6">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6">
-        <v>0.13300000000000001</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="F6">
-        <v>0.246</v>
+        <v>0.16300000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="B7">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7">
-        <v>0.15</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="F7">
-        <v>0.307</v>
+        <v>0.20499999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="B8">
         <v>0.2</v>
@@ -575,15 +575,95 @@
         <v>1</v>
       </c>
       <c r="E8">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="F8">
+        <v>0.20699999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5000</v>
+      </c>
+      <c r="B9">
+        <v>0.3</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="F9">
+        <v>0.22700000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6000</v>
+      </c>
+      <c r="B10">
+        <v>0.15</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="F10">
+        <v>0.246</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5000</v>
+      </c>
+      <c r="B11">
+        <v>0.2</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0.15</v>
+      </c>
+      <c r="F11">
+        <v>0.307</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5000</v>
+      </c>
+      <c r="B12">
+        <v>0.2</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
         <v>0.16500000000000001</v>
       </c>
-      <c r="F8">
+      <c r="F12">
         <v>0.31</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="F1:F7"/>
-  <sortState ref="A2:F8">
+  <sortState ref="A2:F13">
     <sortCondition ref="F1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>